<commit_message>
Major UPD 2, Fixed MANY bugs
</commit_message>
<xml_diff>
--- a/Input/NewData.xlsx
+++ b/Input/NewData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/PHD/Models/Torque-and-Drag/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28EC13E-4876-4CC4-B1B4-9535CBBBFEB1}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB5C6A4C-5CB0-4043-BAF2-4577CEC12235}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SURVEY" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Borehole_Properties" sheetId="12" r:id="rId5"/>
     <sheet name="ADVANCED" sheetId="11" r:id="rId6"/>
     <sheet name="TOP_DRIVE" sheetId="10" r:id="rId7"/>
-    <sheet name="steady_state_inputs" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="steady_state_inputs (2)" sheetId="13" r:id="rId8"/>
+    <sheet name="steady_state_inputs" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>BHA Type</t>
   </si>
@@ -177,88 +178,6 @@
     <t>s</t>
   </si>
   <si>
-    <t>7 5/8" Power Mag Assembly #9 (Riser Mag)</t>
-  </si>
-  <si>
-    <t>1 Stand 23.40# TT-585</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #8 (Riser Mag)</t>
-  </si>
-  <si>
-    <t>27 Stands X 23.40#
-TT-585</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #7</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #6</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #5</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #4</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #3</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #2</t>
-  </si>
-  <si>
-    <t>7 5/8" Power Mag Assembly #1</t>
-  </si>
-  <si>
-    <t>5 Stands XZ3.40# TT-585</t>
-  </si>
-  <si>
-    <t>X-Over Sub</t>
-  </si>
-  <si>
-    <t>10 1/4" BRN Rode Protector</t>
-  </si>
-  <si>
-    <t>29 x 5-7/8" HWDP</t>
-  </si>
-  <si>
-    <t>10 x 8" Drill Collar</t>
-  </si>
-  <si>
-    <t>Downhole Screen</t>
-  </si>
-  <si>
-    <t>8" HOC (Directional &amp; Pulser)</t>
-  </si>
-  <si>
-    <t>8" HCIM Collar</t>
-  </si>
-  <si>
-    <t>8" PWD</t>
-  </si>
-  <si>
-    <t>8" DrillDOC</t>
-  </si>
-  <si>
-    <t>8" Float Sub BFF 5F6R GC</t>
-  </si>
-  <si>
-    <t>SSM 8-in Collar</t>
-  </si>
-  <si>
-    <t>12 1/4" Steering Mill</t>
-  </si>
-  <si>
-    <t>12 1/4" Flex Madrel</t>
-  </si>
-  <si>
-    <t>12 1/4" Secondary Mill</t>
-  </si>
-  <si>
-    <t>12 1/4" Lead Mill</t>
-  </si>
-  <si>
     <t>Number of Items</t>
   </si>
   <si>
@@ -331,9 +250,6 @@
     <t>Stribeck Critical Velocity</t>
   </si>
   <si>
-    <t>ft/s</t>
-  </si>
-  <si>
     <t>ROP steady state</t>
   </si>
   <si>
@@ -349,13 +265,22 @@
     <t>CCS</t>
   </si>
   <si>
-    <t>psi</t>
-  </si>
-  <si>
     <t>ft/hr</t>
   </si>
   <si>
-    <t>lbf-s/in</t>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>N sec/m</t>
+  </si>
+  <si>
+    <t>ksi</t>
+  </si>
+  <si>
+    <t>m/hr</t>
+  </si>
+  <si>
+    <t>COLLAR</t>
   </si>
 </sst>
 </file>
@@ -495,6 +420,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB77188-32FA-43EE-BD2E-FA6085E2DDB4}">
-  <dimension ref="A1:D687"/>
+  <dimension ref="A1:D686"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A121" sqref="A121"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,1918 +739,876 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
+      <c r="A2" s="1">
+        <v>1640.4199475065616</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>A2+200</f>
-        <v>200</v>
+        <v>3280.8398950131232</v>
       </c>
       <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A43" si="0">A3+200</f>
-        <v>400</v>
+        <v>4921.2598425196848</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
-        <v>600</v>
+        <v>6889.7637795275587</v>
       </c>
       <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>800</v>
+        <v>8202.0997375328079</v>
       </c>
       <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>13123.359580052493</v>
       </c>
       <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" si="0"/>
-        <v>1400</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>2200</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>2400</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>2600</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>2800</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>3000</v>
-      </c>
-      <c r="B17" s="9">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <f t="shared" si="0"/>
-        <v>3200</v>
-      </c>
-      <c r="B18" s="9">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
-        <v>3400</v>
-      </c>
-      <c r="B19" s="9">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <f t="shared" si="0"/>
-        <v>3600</v>
-      </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <f t="shared" si="0"/>
-        <v>3800</v>
-      </c>
-      <c r="B21" s="9">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="B22" s="9">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <f t="shared" si="0"/>
-        <v>4200</v>
-      </c>
-      <c r="B23" s="9">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <f t="shared" si="0"/>
-        <v>4400</v>
-      </c>
-      <c r="B24" s="9">
-        <v>0</v>
-      </c>
-      <c r="C24" s="9">
-        <v>0</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="B25" s="9">
-        <v>0</v>
-      </c>
-      <c r="C25" s="9">
-        <v>0</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f t="shared" si="0"/>
-        <v>4800</v>
-      </c>
-      <c r="B26" s="9">
-        <v>0</v>
-      </c>
-      <c r="C26" s="9">
-        <v>0</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <f t="shared" si="0"/>
-        <v>5000</v>
-      </c>
-      <c r="B27" s="9">
-        <v>0</v>
-      </c>
-      <c r="C27" s="9">
-        <v>0</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <f t="shared" si="0"/>
-        <v>5200</v>
-      </c>
-      <c r="B28" s="9">
-        <v>0</v>
-      </c>
-      <c r="C28" s="9">
-        <v>0</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <f t="shared" si="0"/>
-        <v>5400</v>
-      </c>
-      <c r="B29" s="9">
-        <v>0</v>
-      </c>
-      <c r="C29" s="9">
-        <v>0</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <f t="shared" si="0"/>
-        <v>5600</v>
-      </c>
-      <c r="B30" s="9">
-        <v>0</v>
-      </c>
-      <c r="C30" s="9">
-        <v>0</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <f>A30+200</f>
-        <v>5800</v>
-      </c>
-      <c r="B31" s="9">
-        <v>0</v>
-      </c>
-      <c r="C31" s="9">
-        <v>0</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <f t="shared" si="0"/>
-        <v>6000</v>
-      </c>
-      <c r="B32" s="9">
-        <v>0</v>
-      </c>
-      <c r="C32" s="9">
-        <v>0</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>6200</v>
-      </c>
-      <c r="B33" s="9">
-        <v>0</v>
-      </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <f t="shared" si="0"/>
-        <v>6400</v>
-      </c>
-      <c r="B34" s="9">
-        <v>0</v>
-      </c>
-      <c r="C34" s="9">
-        <v>0</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <f t="shared" si="0"/>
-        <v>6600</v>
-      </c>
-      <c r="B35" s="9">
-        <v>0</v>
-      </c>
-      <c r="C35" s="9">
-        <v>0</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <f t="shared" si="0"/>
-        <v>6800</v>
-      </c>
-      <c r="B36" s="9">
-        <v>0</v>
-      </c>
-      <c r="C36" s="9">
-        <v>0</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <f t="shared" si="0"/>
-        <v>7000</v>
-      </c>
-      <c r="B37" s="9">
-        <v>0</v>
-      </c>
-      <c r="C37" s="9">
-        <v>0</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <f t="shared" si="0"/>
-        <v>7200</v>
-      </c>
-      <c r="B38" s="9">
-        <v>0</v>
-      </c>
-      <c r="C38" s="9">
-        <v>0</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <f t="shared" si="0"/>
-        <v>7400</v>
-      </c>
-      <c r="B39" s="9">
-        <v>0</v>
-      </c>
-      <c r="C39" s="9">
-        <v>0</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <f>A39+200</f>
-        <v>7600</v>
-      </c>
-      <c r="B40" s="9">
-        <v>0</v>
-      </c>
-      <c r="C40" s="9">
-        <v>0</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <f t="shared" si="0"/>
-        <v>7800</v>
-      </c>
-      <c r="B41" s="9">
-        <v>0</v>
-      </c>
-      <c r="C41" s="9">
-        <v>0</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="B42" s="9">
-        <v>0</v>
-      </c>
-      <c r="C42" s="9">
-        <v>0</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <f t="shared" si="0"/>
-        <v>8200</v>
-      </c>
-      <c r="B43" s="9">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9">
-        <v>0</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>8381</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="C44" s="11">
-        <v>253.3</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="11"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>8475</v>
-      </c>
-      <c r="B45" s="1">
-        <v>0.22</v>
-      </c>
-      <c r="C45" s="11">
-        <v>257.61</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="11"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>8570</v>
-      </c>
-      <c r="B46" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="C46" s="11">
-        <v>241.46</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="11"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>8664</v>
-      </c>
-      <c r="B47" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="C47" s="11">
-        <v>280.25</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="11"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>8758</v>
-      </c>
-      <c r="B48" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="C48" s="11">
-        <v>253.62</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>8852</v>
-      </c>
-      <c r="B49" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="C49" s="11">
-        <v>239.95</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="11"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>8947</v>
-      </c>
-      <c r="B50" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="C50" s="11">
-        <v>263.43</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="11"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>9041</v>
-      </c>
-      <c r="B51" s="1">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="C51" s="11">
-        <v>240.49</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="11"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>9135</v>
-      </c>
-      <c r="B52" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="C52" s="11">
-        <v>293.62</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="11"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>9229</v>
-      </c>
-      <c r="B53" s="1">
-        <v>1.08</v>
-      </c>
-      <c r="C53" s="11">
-        <v>301.02999999999997</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="11"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>9313</v>
-      </c>
-      <c r="B54" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="C54" s="11">
-        <v>283.72000000000003</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="11"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>9407</v>
-      </c>
-      <c r="B55" s="1">
-        <v>1.86</v>
-      </c>
-      <c r="C55" s="11">
-        <v>334.4</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="11"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>9502</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1.58</v>
-      </c>
-      <c r="C56" s="11">
-        <v>322.02999999999997</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="11"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>9596</v>
-      </c>
-      <c r="B57" s="1">
-        <v>3.36</v>
-      </c>
-      <c r="C57" s="11">
-        <v>338.6</v>
-      </c>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="11"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>9690</v>
-      </c>
-      <c r="B58" s="1">
-        <v>4.03</v>
-      </c>
-      <c r="C58" s="11">
-        <v>353.4</v>
-      </c>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="11"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>9784</v>
-      </c>
-      <c r="B59" s="1">
-        <v>7.1</v>
-      </c>
-      <c r="C59" s="11">
-        <v>355.99</v>
-      </c>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>9879</v>
-      </c>
-      <c r="B60" s="1">
-        <v>9.02</v>
-      </c>
-      <c r="C60" s="11">
-        <v>358.51</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="11"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>9973</v>
-      </c>
-      <c r="B61" s="1">
-        <v>11.52</v>
-      </c>
-      <c r="C61" s="11">
-        <v>355.3</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="11"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>10067</v>
-      </c>
-      <c r="B62" s="1">
-        <v>14.04</v>
-      </c>
-      <c r="C62" s="11">
-        <v>350.61</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="11"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>10161</v>
-      </c>
-      <c r="B63" s="1">
-        <v>15.16</v>
-      </c>
-      <c r="C63" s="11">
-        <v>352.1</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="11"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>10257</v>
-      </c>
-      <c r="B64" s="1">
-        <v>19.57</v>
-      </c>
-      <c r="C64" s="11">
-        <v>354.44</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="11"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>10350</v>
-      </c>
-      <c r="B65" s="1">
-        <v>22.11</v>
-      </c>
-      <c r="C65" s="11">
-        <v>355.54</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="11"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>10444</v>
-      </c>
-      <c r="B66" s="1">
-        <v>22.69</v>
-      </c>
-      <c r="C66" s="11">
-        <v>352.99</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="11"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>10539</v>
-      </c>
-      <c r="B67" s="1">
-        <v>25.47</v>
-      </c>
-      <c r="C67" s="11">
-        <v>349.72</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="11"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>10633</v>
-      </c>
-      <c r="B68" s="1">
-        <v>26.58</v>
-      </c>
-      <c r="C68" s="11">
-        <v>350.95</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>10700</v>
-      </c>
-      <c r="B69" s="1">
-        <v>27.63</v>
-      </c>
-      <c r="C69" s="11">
-        <v>350.81</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="11"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>10764</v>
-      </c>
-      <c r="B70" s="1">
-        <v>27.18</v>
-      </c>
-      <c r="C70" s="11">
-        <v>352.26</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>10858</v>
-      </c>
-      <c r="B71" s="1">
-        <v>28.33</v>
-      </c>
-      <c r="C71" s="11">
-        <v>352.99</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="11"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>10953</v>
-      </c>
-      <c r="B72" s="1">
-        <v>31.98</v>
-      </c>
-      <c r="C72" s="11">
-        <v>353.69</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="11"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>11048</v>
-      </c>
-      <c r="B73" s="1">
-        <v>34.450000000000003</v>
-      </c>
-      <c r="C73" s="11">
-        <v>353.67</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="11"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>11142</v>
-      </c>
-      <c r="B74" s="1">
-        <v>35.590000000000003</v>
-      </c>
-      <c r="C74" s="11">
-        <v>354.12</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="11"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>11236</v>
-      </c>
-      <c r="B75" s="1">
-        <v>38.4</v>
-      </c>
-      <c r="C75" s="11">
-        <v>354.66</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="11"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>11331</v>
-      </c>
-      <c r="B76" s="1">
-        <v>40.79</v>
-      </c>
-      <c r="C76" s="11">
-        <v>355.24</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="11"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>11425</v>
-      </c>
-      <c r="B77" s="1">
-        <v>43.82</v>
-      </c>
-      <c r="C77" s="11">
-        <v>355.23</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>11517</v>
-      </c>
-      <c r="B78" s="1">
-        <v>46.28</v>
-      </c>
-      <c r="C78" s="11">
-        <v>356.21</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="11"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>11615</v>
-      </c>
-      <c r="B79" s="1">
-        <v>49.61</v>
-      </c>
-      <c r="C79" s="11">
-        <v>356.91</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="11"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>11709</v>
-      </c>
-      <c r="B80" s="1">
-        <v>52.61</v>
-      </c>
-      <c r="C80" s="11">
-        <v>356.44</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="11"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>11804</v>
-      </c>
-      <c r="B81" s="1">
-        <v>55.21</v>
-      </c>
-      <c r="C81" s="11">
-        <v>356.22</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="11"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>11899</v>
-      </c>
-      <c r="B82" s="1">
-        <v>57.64</v>
-      </c>
-      <c r="C82" s="11">
-        <v>356.03</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="11"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>11993</v>
-      </c>
-      <c r="B83" s="1">
-        <v>61.45</v>
-      </c>
-      <c r="C83" s="11">
-        <v>356.27</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="11"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>12088</v>
-      </c>
-      <c r="B84" s="1">
-        <v>64.5</v>
-      </c>
-      <c r="C84" s="11">
-        <v>357.32</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="11"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
-        <v>12182</v>
-      </c>
-      <c r="B85" s="1">
-        <v>67.400000000000006</v>
-      </c>
-      <c r="C85" s="11">
-        <v>357.73</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="11"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
-        <v>12277</v>
-      </c>
-      <c r="B86" s="1">
-        <v>69.91</v>
-      </c>
-      <c r="C86" s="11">
-        <v>357.94</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="11"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
-        <v>12372</v>
-      </c>
-      <c r="B87" s="1">
-        <v>68.52</v>
-      </c>
-      <c r="C87" s="11">
-        <v>358.05</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="11"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>12466</v>
-      </c>
-      <c r="B88" s="1">
-        <v>67.59</v>
-      </c>
-      <c r="C88" s="11">
-        <v>357.96</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="11"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>12503</v>
-      </c>
-      <c r="B89" s="1">
-        <v>68.459999999999994</v>
-      </c>
-      <c r="C89" s="11">
-        <v>359.41</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="11"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>12591</v>
-      </c>
-      <c r="B90" s="1">
-        <v>68.900000000000006</v>
-      </c>
-      <c r="C90" s="11">
-        <v>0.99</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="11"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>12686</v>
-      </c>
-      <c r="B91" s="1">
-        <v>70.22</v>
-      </c>
-      <c r="C91" s="11">
-        <v>2.0499999999999998</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="11"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>12780</v>
-      </c>
-      <c r="B92" s="1">
-        <v>71.010000000000005</v>
-      </c>
-      <c r="C92" s="11">
-        <v>3.99</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="11"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
-        <v>12874</v>
-      </c>
-      <c r="B93" s="1">
-        <v>71.010000000000005</v>
-      </c>
-      <c r="C93" s="11">
-        <v>6.31</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="11"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>12954</v>
-      </c>
-      <c r="B94" s="1">
-        <v>70.34</v>
-      </c>
-      <c r="C94" s="11">
-        <v>8.0299999999999994</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="11"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
-        <v>13048</v>
-      </c>
-      <c r="B95" s="1">
-        <v>70.58</v>
-      </c>
-      <c r="C95" s="11">
-        <v>9.19</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="11"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>13143</v>
-      </c>
-      <c r="B96" s="1">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="C96" s="11">
-        <v>10.43</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="11"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
-        <v>13237</v>
-      </c>
-      <c r="B97" s="1">
-        <v>71.17</v>
-      </c>
-      <c r="C97" s="11">
-        <v>11.92</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="11"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
-        <v>13332</v>
-      </c>
-      <c r="B98" s="1">
-        <v>71.47</v>
-      </c>
-      <c r="C98" s="11">
-        <v>13.34</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="11"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
-        <v>13425</v>
-      </c>
-      <c r="B99" s="1">
-        <v>71.53</v>
-      </c>
-      <c r="C99" s="11">
-        <v>14.14</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="11"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
-        <v>13520.000000000002</v>
-      </c>
-      <c r="B100" s="1">
-        <v>72.19</v>
-      </c>
-      <c r="C100" s="11">
-        <v>15.4</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="11"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
-        <v>13613</v>
-      </c>
-      <c r="B101" s="1">
-        <v>72.5</v>
-      </c>
-      <c r="C101" s="11">
-        <v>18.05</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="11"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
-        <v>13709</v>
-      </c>
-      <c r="B102" s="1">
-        <v>72.739999999999995</v>
-      </c>
-      <c r="C102" s="11">
-        <v>20.09</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="11"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
-        <v>13806</v>
-      </c>
-      <c r="B103" s="1">
-        <v>73.180000000000007</v>
-      </c>
-      <c r="C103" s="11">
-        <v>21.86</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="11"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
-        <v>13901</v>
-      </c>
-      <c r="B104" s="1">
-        <v>74.44</v>
-      </c>
-      <c r="C104" s="11">
-        <v>23.94</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="11"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
-        <v>13995</v>
-      </c>
-      <c r="B105" s="1">
-        <v>75.430000000000007</v>
-      </c>
-      <c r="C105" s="11">
-        <v>26.06</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="11"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
-        <v>14089.000000000002</v>
-      </c>
-      <c r="B106" s="1">
-        <v>76.23</v>
-      </c>
-      <c r="C106" s="11">
-        <v>27.43</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="11"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
-        <v>14183.999999999998</v>
-      </c>
-      <c r="B107" s="1">
-        <v>76.739999999999995</v>
-      </c>
-      <c r="C107" s="11">
-        <v>27.74</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="11"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
-        <v>14378.000000000002</v>
-      </c>
-      <c r="B108" s="1">
-        <v>76.77</v>
-      </c>
-      <c r="C108" s="11">
-        <v>27.58</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="11"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
-        <v>14464.999999999998</v>
-      </c>
-      <c r="B109" s="1">
-        <v>76.86</v>
-      </c>
-      <c r="C109" s="11">
-        <v>27.33</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="11"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
-        <v>14558</v>
-      </c>
-      <c r="B110" s="1">
-        <v>76.77</v>
-      </c>
-      <c r="C110" s="11">
-        <v>27.55</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="11"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
-        <v>14650.000000000002</v>
-      </c>
-      <c r="B111" s="1">
-        <v>76.95</v>
-      </c>
-      <c r="C111" s="11">
-        <v>27.79</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="11"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
-        <v>14744</v>
-      </c>
-      <c r="B112" s="1">
-        <v>76.89</v>
-      </c>
-      <c r="C112" s="11">
-        <v>28.19</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="11"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
-        <v>14838</v>
-      </c>
-      <c r="B113" s="1">
-        <v>76.33</v>
-      </c>
-      <c r="C113" s="11">
-        <v>27.91</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="11"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
-        <v>14930.000000000002</v>
-      </c>
-      <c r="B114" s="1">
-        <v>76.260000000000005</v>
-      </c>
-      <c r="C114" s="11">
-        <v>27.4</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="11"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
-        <v>15024</v>
-      </c>
-      <c r="B115" s="1">
-        <v>76.23</v>
-      </c>
-      <c r="C115" s="11">
-        <v>27.36</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="11"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
-        <v>15117</v>
-      </c>
-      <c r="B116" s="1">
-        <v>76.569999999999993</v>
-      </c>
-      <c r="C116" s="11">
-        <v>27.83</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="11"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="1">
-        <v>15209.999999999998</v>
-      </c>
-      <c r="B117" s="1">
-        <v>76.52</v>
-      </c>
-      <c r="C117" s="11">
-        <v>27.91</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="11"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="1">
-        <v>15303</v>
-      </c>
-      <c r="B118" s="1">
-        <v>76.39</v>
-      </c>
-      <c r="C118" s="11">
-        <v>28.1</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="11"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
-        <v>15396.000000000002</v>
-      </c>
-      <c r="B119" s="1">
-        <v>76.55</v>
-      </c>
-      <c r="C119" s="11">
-        <v>28.39</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="11"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="1">
-        <v>15489</v>
-      </c>
-      <c r="B120" s="1">
-        <v>76.67</v>
-      </c>
-      <c r="C120" s="11">
-        <v>28.51</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="11"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="1">
-        <v>15582</v>
-      </c>
-      <c r="B121" s="1">
-        <v>76.739999999999995</v>
-      </c>
-      <c r="C121" s="11">
-        <v>28.6</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="11"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1">
-        <v>15676.000000000002</v>
-      </c>
-      <c r="B122" s="1">
-        <v>76.64</v>
-      </c>
-      <c r="C122" s="11">
-        <v>28.4</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="11"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>15769</v>
-      </c>
-      <c r="B123" s="1">
-        <v>76.55</v>
-      </c>
-      <c r="C123" s="11">
-        <v>28.35</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="11"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1">
-        <v>15862</v>
-      </c>
-      <c r="B124" s="1">
-        <v>76.510000000000005</v>
-      </c>
-      <c r="C124" s="11">
-        <v>28.74</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="11"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1">
-        <v>15954.999999999998</v>
-      </c>
-      <c r="B125" s="1">
-        <v>76.36</v>
-      </c>
-      <c r="C125" s="11">
-        <v>28.66</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="11"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1">
-        <v>16048</v>
-      </c>
-      <c r="B126" s="1">
-        <v>76.23</v>
-      </c>
-      <c r="C126" s="11">
-        <v>28.61</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="11"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
-        <v>16141.000000000002</v>
-      </c>
-      <c r="B127" s="1">
-        <v>75.930000000000007</v>
-      </c>
-      <c r="C127" s="11">
-        <v>28.93</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="11"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
-        <v>16234</v>
-      </c>
-      <c r="B128" s="1">
-        <v>76.319999999999993</v>
-      </c>
-      <c r="C128" s="11">
-        <v>28.8</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="11"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="1">
-        <v>16327</v>
-      </c>
-      <c r="B129" s="1">
-        <v>76.17</v>
-      </c>
-      <c r="C129" s="11">
-        <v>28.75</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="11"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="1">
-        <v>16420</v>
-      </c>
-      <c r="B130" s="1">
-        <v>76.23</v>
-      </c>
-      <c r="C130" s="11">
-        <v>28.5</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="11"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="1">
-        <v>16513</v>
-      </c>
-      <c r="B131" s="1">
-        <v>76.36</v>
-      </c>
-      <c r="C131" s="11">
-        <v>28.4</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="11"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>16605</v>
-      </c>
-      <c r="B132" s="1">
-        <v>76.67</v>
-      </c>
-      <c r="C132" s="11">
-        <v>28.77</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="11"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>16699</v>
-      </c>
-      <c r="B133" s="1">
-        <v>76.290000000000006</v>
-      </c>
-      <c r="C133" s="11">
-        <v>28.31</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="11"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="1">
-        <v>16793</v>
-      </c>
-      <c r="B134" s="1">
-        <v>76.33</v>
-      </c>
-      <c r="C134" s="11">
-        <v>28.38</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="11"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1">
-        <v>16886</v>
-      </c>
-      <c r="B135" s="1">
-        <v>76.45</v>
-      </c>
-      <c r="C135" s="11">
-        <v>28.4</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="11"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="1">
-        <v>16978</v>
-      </c>
-      <c r="B136" s="1">
-        <v>76.38</v>
-      </c>
-      <c r="C136" s="11">
-        <v>28.25</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="11"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>17070</v>
-      </c>
-      <c r="B137" s="1">
-        <v>76.39</v>
-      </c>
-      <c r="C137" s="11">
-        <v>28.12</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="11"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <v>17163</v>
-      </c>
-      <c r="B138" s="1">
-        <v>76.23</v>
-      </c>
-      <c r="C138" s="11">
-        <v>28.29</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="11"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>17256</v>
-      </c>
-      <c r="B139" s="1">
-        <v>76.319999999999993</v>
-      </c>
-      <c r="C139" s="11">
-        <v>28.57</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="11"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="1">
-        <v>17349</v>
-      </c>
-      <c r="B140" s="1">
-        <v>75.88</v>
-      </c>
-      <c r="C140" s="11">
-        <v>29.55</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="11"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="1">
-        <v>17442</v>
-      </c>
-      <c r="B141" s="1">
-        <v>75.97</v>
-      </c>
-      <c r="C141" s="11">
-        <v>30.92</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="11"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
-        <v>17535</v>
-      </c>
-      <c r="B142" s="1">
-        <v>75.62</v>
-      </c>
-      <c r="C142" s="11">
-        <v>31.85</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="11"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
-        <v>17628</v>
-      </c>
-      <c r="B143" s="1">
-        <v>75.209999999999994</v>
-      </c>
-      <c r="C143" s="11">
-        <v>32.92</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="11"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>17721</v>
-      </c>
-      <c r="B144" s="1">
-        <v>74.83</v>
-      </c>
-      <c r="C144" s="11">
-        <v>33.869999999999997</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="11"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>17814</v>
-      </c>
-      <c r="B145" s="1">
-        <v>74.7</v>
-      </c>
-      <c r="C145" s="11">
-        <v>34.67</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="11"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>17909</v>
-      </c>
-      <c r="B146" s="1">
-        <v>74.349999999999994</v>
-      </c>
-      <c r="C146" s="11">
-        <v>35.25</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="11"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
-        <v>18002</v>
-      </c>
-      <c r="B147" s="1">
-        <v>74.28</v>
-      </c>
-      <c r="C147" s="11">
-        <v>35.26</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="11"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>18095</v>
-      </c>
-      <c r="B148" s="1">
-        <v>71.95</v>
-      </c>
-      <c r="C148" s="11">
-        <v>35.39</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="11"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="1">
-        <v>18188</v>
-      </c>
-      <c r="B149" s="1">
-        <v>70.010000000000005</v>
-      </c>
-      <c r="C149" s="11">
-        <v>36.15</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="11"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
-        <v>18282</v>
-      </c>
-      <c r="B150" s="1">
-        <v>67.66</v>
-      </c>
-      <c r="C150" s="11">
-        <v>37.75</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="11"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
-        <v>18375</v>
-      </c>
-      <c r="B151" s="1">
-        <v>65.87</v>
-      </c>
-      <c r="C151" s="11">
-        <v>38.47</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="11"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="1">
-        <v>18469</v>
-      </c>
-      <c r="B152" s="1">
-        <v>63</v>
-      </c>
-      <c r="C152" s="11">
-        <v>39.08</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="11"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="1">
-        <v>18562</v>
-      </c>
-      <c r="B153" s="1">
-        <v>60.53</v>
-      </c>
-      <c r="C153" s="11">
-        <v>40.67</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="11"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="1">
-        <v>18655</v>
-      </c>
-      <c r="B154" s="1">
-        <v>58.37</v>
-      </c>
-      <c r="C154" s="11">
-        <v>42.77</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="11"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
-        <v>18748</v>
-      </c>
-      <c r="B155" s="1">
-        <v>56.25</v>
-      </c>
-      <c r="C155" s="11">
-        <v>43.27</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="11"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="1">
-        <v>18841</v>
-      </c>
-      <c r="B156" s="1">
-        <v>54.13</v>
-      </c>
-      <c r="C156" s="11">
-        <v>44.12</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="11"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="1">
-        <v>18934</v>
-      </c>
-      <c r="B157" s="1">
-        <v>52.14</v>
-      </c>
-      <c r="C157" s="11">
-        <v>44.73</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="11"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
-        <v>19041</v>
-      </c>
-      <c r="B158" s="1">
-        <v>49.99</v>
-      </c>
-      <c r="C158" s="11">
-        <v>45.19</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="11"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
-        <v>19134</v>
-      </c>
-      <c r="B159" s="1">
-        <v>48.66</v>
-      </c>
-      <c r="C159" s="11">
-        <v>47.82</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="11"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="1">
-        <v>19227</v>
-      </c>
-      <c r="B160" s="1">
-        <v>47.2</v>
-      </c>
-      <c r="C160" s="11">
-        <v>50.06</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="11"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
-        <v>19321</v>
-      </c>
-      <c r="B161" s="1">
-        <v>45.07</v>
-      </c>
-      <c r="C161" s="11">
-        <v>52.58</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="11"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
-        <v>19414</v>
-      </c>
-      <c r="B162" s="1">
-        <v>43.42</v>
-      </c>
-      <c r="C162" s="11">
-        <v>54.61</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="11"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="1">
-        <v>19507</v>
-      </c>
-      <c r="B163" s="1">
-        <v>41.74</v>
-      </c>
-      <c r="C163" s="11">
-        <v>57.08</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="11"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
-        <v>19600</v>
-      </c>
-      <c r="B164" s="1">
-        <v>40.04</v>
-      </c>
-      <c r="C164" s="11">
-        <v>60.06</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="11"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
-        <v>19693</v>
-      </c>
-      <c r="B165" s="1">
-        <v>38.72</v>
-      </c>
-      <c r="C165" s="11">
-        <v>63.59</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="11"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="1">
-        <v>19786</v>
-      </c>
-      <c r="B166" s="1">
-        <v>36.909999999999997</v>
-      </c>
-      <c r="C166" s="11">
-        <v>66.739999999999995</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="11"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="1">
-        <v>19879</v>
-      </c>
-      <c r="B167" s="1">
-        <v>35.79</v>
-      </c>
-      <c r="C167" s="11">
-        <v>67.680000000000007</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="11"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="1">
-        <v>19910</v>
-      </c>
-      <c r="B168" s="1">
-        <v>35.72</v>
-      </c>
-      <c r="C168" s="11">
-        <v>68.209999999999994</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="11"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
-        <v>19994</v>
-      </c>
-      <c r="B169" s="1">
-        <v>35.6</v>
-      </c>
-      <c r="C169" s="11">
-        <v>69</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="11"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="1">
-        <v>20087</v>
-      </c>
-      <c r="B170" s="1">
-        <v>35.64</v>
-      </c>
-      <c r="C170" s="11">
-        <v>69.31</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="11"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="1">
-        <v>20185</v>
-      </c>
-      <c r="B171" s="1">
-        <v>35.64</v>
-      </c>
-      <c r="C171" s="11">
-        <v>69.31</v>
-      </c>
+      <c r="C171" s="5"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C172" s="5"/>
@@ -4267,9 +3154,6 @@
     </row>
     <row r="686" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C686" s="5"/>
-    </row>
-    <row r="687" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C687" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4281,7 +3165,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4301,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -4336,23 +3220,24 @@
         <v>11</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>94.65</v>
+        <f>40/0.3048</f>
+        <v>131.23359580052494</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E30" si="0">E3+D2</f>
-        <v>4883.7899999999991</v>
+        <f t="shared" ref="E2:E4" si="0">E3+D2</f>
+        <v>323.58923884514434</v>
       </c>
       <c r="F2" s="1">
         <v>5.875</v>
       </c>
       <c r="G2" s="1">
-        <v>5.1529999999999996</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -4361,11 +3246,11 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <f>26.87*D2</f>
-        <v>2543.2455000000004</v>
+        <f>25.62*D2</f>
+        <v>3362.2047244094492</v>
       </c>
       <c r="K2" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>13</v>
@@ -4373,26 +3258,27 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="6">
-        <v>47.65</v>
+        <f>28.63/0.3048</f>
+        <v>93.930446194225709</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>4789.1399999999994</v>
+        <v>192.3556430446194</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>5.88</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -4401,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>5089.0199999999995</v>
+        <v>2406.545510333317</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -4415,23 +3301,24 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="6">
-        <v>94.65</v>
+        <f>30/0.3048</f>
+        <v>98.425196850393689</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>4741.49</v>
+        <v>98.425196850393689</v>
       </c>
       <c r="F4">
-        <v>5.875</v>
+        <v>5.88</v>
       </c>
       <c r="G4">
-        <v>5.1529999999999996</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -4440,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2543.2455000000004</v>
+        <v>2521.7032940970839</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -4450,1057 +3337,220 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6">
-        <v>47.77</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4646.84</v>
-      </c>
-      <c r="F5">
-        <v>7.6139999999999999</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>5101.8360000000002</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="13"/>
+      <c r="C5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="1">
-        <v>27</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2553.34</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>4599.07</v>
-      </c>
-      <c r="F6">
-        <v>5.875</v>
-      </c>
-      <c r="G6">
-        <v>5.1529999999999996</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>68608.245800000004</v>
-      </c>
-      <c r="K6" s="1">
-        <v>5</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="13"/>
+      <c r="C6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6">
-        <v>41.7</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>2045.73</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>4453.5600000000004</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="13"/>
+      <c r="C7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6">
-        <v>38.950000000000003</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>2004.03</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>4159.8600000000006</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A8" s="13"/>
+      <c r="C8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6">
-        <v>39.15</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1965.08</v>
-      </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>4181.2199999999993</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A9" s="13"/>
+      <c r="C9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1925.9299999999998</v>
-      </c>
-      <c r="F10">
-        <v>7.33</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>4090.4399999999996</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A10" s="13"/>
+      <c r="C10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="6">
-        <v>40.869999999999997</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1887.6299999999999</v>
-      </c>
-      <c r="F11">
-        <v>7.33</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>4364.9159999999993</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A11" s="13"/>
+      <c r="C11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="6">
-        <v>38.369999999999997</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1846.76</v>
-      </c>
-      <c r="F12">
-        <v>7.4</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>4097.9159999999993</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A12" s="13"/>
+      <c r="C12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>40.96</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1808.39</v>
-      </c>
-      <c r="F13">
-        <v>7.4</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>4374.5280000000002</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A13" s="13"/>
+      <c r="C13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="1">
-        <v>5</v>
-      </c>
-      <c r="D14" s="6">
-        <v>474.18</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1767.43</v>
-      </c>
-      <c r="F14">
-        <v>5.875</v>
-      </c>
-      <c r="G14">
-        <v>5.1529999999999996</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>12741.216600000002</v>
-      </c>
-      <c r="K14" s="1">
-        <v>5</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="13"/>
+      <c r="C14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6">
-        <v>4.53</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1293.25</v>
-      </c>
-      <c r="F15">
-        <v>8.31</v>
-      </c>
-      <c r="G15">
-        <v>3.25</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>710.62110000000007</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="13"/>
+      <c r="C15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1288.72</v>
-      </c>
-      <c r="F16">
-        <v>8.25</v>
-      </c>
-      <c r="G16">
-        <v>3.25</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>752.61989999999992</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A16" s="13"/>
+      <c r="C16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6">
-        <v>3.62</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1283.83</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
-      </c>
-      <c r="G17">
-        <v>3.5</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>501.44240000000008</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A17" s="13"/>
+      <c r="C17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="1">
-        <v>29</v>
-      </c>
-      <c r="D18" s="6">
-        <v>876.1400000000001</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1280.21</v>
-      </c>
-      <c r="F18">
-        <v>5.875</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>49878.650199999996</v>
-      </c>
-      <c r="K18" s="1">
-        <v>5</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A18" s="13"/>
+      <c r="C18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>404.07000000000005</v>
-      </c>
-      <c r="F19">
-        <v>8</v>
-      </c>
-      <c r="G19">
-        <v>3.5</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>346.3</v>
-      </c>
-      <c r="K19" s="1">
-        <v>0</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A19" s="13"/>
+      <c r="C19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1">
-        <v>10</v>
-      </c>
-      <c r="D20" s="6">
-        <v>294.74</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>401.57000000000005</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-      <c r="G20">
-        <v>2.8130000000000002</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>44246.368800000004</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A20" s="13"/>
+      <c r="C20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>106.83000000000001</v>
-      </c>
-      <c r="F21">
-        <v>8</v>
-      </c>
-      <c r="G21">
-        <v>2.8130000000000002</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>1418.634</v>
-      </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A21" s="13"/>
+      <c r="C21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6">
-        <v>15.12</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>97.38000000000001</v>
-      </c>
-      <c r="F22">
-        <v>8.15</v>
-      </c>
-      <c r="G22">
-        <v>1.92</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>2286.1439999999998</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A22" s="13"/>
+      <c r="C22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="6">
-        <v>7.7</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>82.26</v>
-      </c>
-      <c r="F23">
-        <v>8</v>
-      </c>
-      <c r="G23">
-        <v>1.92</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>1154.23</v>
-      </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A23" s="13"/>
+      <c r="C23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6">
-        <v>7.6599999999999993</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>74.56</v>
-      </c>
-      <c r="F24">
-        <v>8</v>
-      </c>
-      <c r="G24">
-        <v>1.92</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>1098.444</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="A24" s="13"/>
+      <c r="C24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>66.900000000000006</v>
-      </c>
-      <c r="F25">
-        <v>8.2189999999999994</v>
-      </c>
-      <c r="G25">
-        <v>2.37</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>926.90550000000007</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A25" s="13"/>
+      <c r="C25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6">
-        <v>2.46</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>58.35</v>
-      </c>
-      <c r="F26">
-        <v>8</v>
-      </c>
-      <c r="G26">
-        <v>2.8130000000000002</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>369.29520000000002</v>
-      </c>
-      <c r="K26" s="1">
-        <v>0</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A26" s="13"/>
+      <c r="C26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="6">
-        <v>30.42</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>55.89</v>
-      </c>
-      <c r="F27">
-        <v>8</v>
-      </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-      <c r="J27">
-        <v>4885.4520000000002</v>
-      </c>
-      <c r="K27" s="1">
-        <v>0</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="13"/>
+      <c r="C27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="6">
-        <v>3.67</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>25.47</v>
-      </c>
-      <c r="F28">
-        <v>7.5</v>
-      </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>464.14490000000001</v>
-      </c>
-      <c r="K28" s="1">
-        <v>0</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A28" s="13"/>
+      <c r="C28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6">
-        <v>11.96</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>21.8</v>
-      </c>
-      <c r="F29">
-        <v>5.75</v>
-      </c>
-      <c r="G29">
-        <v>3</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>359.7568</v>
-      </c>
-      <c r="K29" s="1">
-        <v>0</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A29" s="13"/>
+      <c r="C29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="6">
-        <v>7.29</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>9.84</v>
-      </c>
-      <c r="F30">
-        <v>7.5</v>
-      </c>
-      <c r="G30">
-        <v>3</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>921.96630000000005</v>
-      </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A30" s="13"/>
+      <c r="C30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="6">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="E31">
-        <f>D31</f>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F31">
-        <v>8</v>
-      </c>
-      <c r="G31">
-        <v>2.8130000000000002</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <v>0</v>
-      </c>
-      <c r="J31">
-        <v>382.80599999999998</v>
-      </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A31" s="13"/>
+      <c r="C31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6434,7 +4484,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6461,7 +4511,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="1">
-        <v>9.4</v>
+        <v>13.436</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
@@ -6502,44 +4552,43 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="B6" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B7" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1">
-        <f>0.03/0.3048</f>
-        <v>9.8425196850393692E-2</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1">
-        <f>15000/4.4482216</f>
-        <v>3372.1341580644271</v>
+        <f>15000</f>
+        <v>15000</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6564,7 +4613,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6602,7 +4651,8 @@
         <v>39</v>
       </c>
       <c r="B3" s="1">
-        <v>20185</v>
+        <f>4000/0.3048</f>
+        <v>13123.359580052493</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>40</v>
@@ -6613,7 +4663,8 @@
         <v>36</v>
       </c>
       <c r="B4" s="6">
-        <v>60808000000</v>
+        <f>60800000000</f>
+        <v>60800000000</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>37</v>
@@ -6621,9 +4672,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="10">
+        <v>65</v>
+      </c>
+      <c r="B5" s="6">
+        <f>210000000000</f>
         <v>210000000000</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -6632,13 +4684,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="B6" s="15">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6674,7 +4726,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,130 +4744,130 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B2" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B3" s="6">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B5" s="6">
-        <v>50</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B6" s="6">
-        <v>60</v>
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="B7" s="6">
-        <v>70</v>
+        <v>400</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="B8" s="6">
-        <v>110</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6">
-        <v>120</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B10" s="6">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="B11" s="6">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B12" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6">
-        <v>50</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="B14" s="6">
-        <v>60</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B15" s="6">
-        <v>70</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="B16" s="6">
-        <v>110</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B17" s="6">
-        <v>120</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -6824,6 +4876,131 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F0C45D-A8D2-4BB4-8B99-E7B938DCB392}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F923E49D-3BBC-49B4-9B07-9E9EA57DE157}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -6852,29 +5029,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1">
         <v>120</v>

</xml_diff>

<commit_message>
Major UPD | * Added new functions with new calcs * Added .gitignore * Removed unnecessary files * Changed calculations to SI units etc.
</commit_message>
<xml_diff>
--- a/Input/NewData.xlsx
+++ b/Input/NewData.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/PHD/Models/Model_v2.0/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/PHD/Models/Torque-and-Drag/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{92381814-82D4-4EE5-A297-684D07C9B3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DFF464B-90CC-4138-9012-F6B50D929875}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{92381814-82D4-4EE5-A297-684D07C9B3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2127465A-E6A8-44D8-9699-7873305F1326}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32355" yWindow="1245" windowWidth="21600" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SURVEY" sheetId="5" r:id="rId1"/>
     <sheet name="BHA" sheetId="1" r:id="rId2"/>
     <sheet name="BHA_REST1" sheetId="7" state="hidden" r:id="rId3"/>
     <sheet name="BHA_REST2" sheetId="8" state="hidden" r:id="rId4"/>
-    <sheet name="ADVANCED" sheetId="9" r:id="rId5"/>
+    <sheet name="Borehole_Properties" sheetId="11" r:id="rId5"/>
+    <sheet name="ADVANCED" sheetId="9" r:id="rId6"/>
+    <sheet name="PUMP" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="46">
   <si>
     <t>BHA Type</t>
   </si>
@@ -153,15 +155,6 @@
     <t>in</t>
   </si>
   <si>
-    <t>Young's Modulus</t>
-  </si>
-  <si>
-    <t>Bulk Modulus</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
     <t>Mud Density</t>
   </si>
   <si>
@@ -174,10 +167,19 @@
     <t>Steel Density</t>
   </si>
   <si>
-    <t>Run Time</t>
+    <t>Number of Items</t>
   </si>
   <si>
-    <t>s</t>
+    <t>Element Length</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Flow Rate</t>
+  </si>
+  <si>
+    <t>GPM</t>
   </si>
 </sst>
 </file>
@@ -577,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB77188-32FA-43EE-BD2E-FA6085E2DDB4}">
   <dimension ref="A1:D688"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H363" sqref="H363"/>
+    <sheetView tabSelected="1" topLeftCell="A659" workbookViewId="0">
+      <selection activeCell="A688" sqref="A688"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10222,10 +10224,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10236,7 +10238,7 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -10244,358 +10246,406 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <f>31.5*C2</f>
         <v>31.5</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:E9" si="0">E3+D2</f>
+        <v>130.80000000000001</v>
+      </c>
+      <c r="F2" s="1">
         <v>5.5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>4.78</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G8" si="0">C2+G3</f>
-        <v>130.80000000000001</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>816.79*C2</f>
         <v>816.79</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>3.84*C3</f>
         <v>3.84</v>
       </c>
-      <c r="D3" s="1">
-        <v>7.27</v>
-      </c>
       <c r="E3" s="1">
-        <v>2.75</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
         <f t="shared" si="0"/>
         <v>99.3</v>
       </c>
+      <c r="F3" s="1">
+        <v>7.27</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.75</v>
+      </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f>465.52*C3</f>
         <v>465.52</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <f>4.26*C4</f>
         <v>4.26</v>
       </c>
-      <c r="D4" s="1">
-        <v>6.75</v>
-      </c>
       <c r="E4" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>95.46</v>
       </c>
+      <c r="F4" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.25</v>
+      </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f>399.08*C4</f>
         <v>399.08</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f>4.12*C5</f>
         <v>4.12</v>
       </c>
-      <c r="D5" s="1">
-        <v>6.75</v>
-      </c>
       <c r="E5" s="1">
-        <v>2.75</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>91.199999999999989</v>
       </c>
+      <c r="F5" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2.75</v>
+      </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <f>419.05*C5</f>
         <v>419.05</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f>14.92*C6</f>
         <v>14.92</v>
       </c>
-      <c r="D6" s="1">
-        <v>6.75</v>
-      </c>
       <c r="E6" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
         <f t="shared" si="0"/>
         <v>87.079999999999984</v>
       </c>
+      <c r="F6" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.25</v>
+      </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <f>1397.71*C6</f>
         <v>1397.71</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f>6.71*C7</f>
         <v>6.71</v>
       </c>
-      <c r="D7" s="1">
-        <v>6.75</v>
-      </c>
       <c r="E7" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>72.159999999999982</v>
       </c>
+      <c r="F7" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3.25</v>
+      </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <f>628.59*C7</f>
         <v>628.59</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f>29.15*C8</f>
         <v>29.15</v>
       </c>
-      <c r="D8" s="1">
-        <v>6.75</v>
-      </c>
       <c r="E8" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
         <f t="shared" si="0"/>
         <v>65.449999999999989</v>
       </c>
+      <c r="F8" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3.25</v>
+      </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f>2730.77*C8</f>
         <v>2730.77</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f>35.3*C9</f>
         <v>35.299999999999997</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="E9" s="1">
+      <c r="G9" s="1">
         <v>3.25</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f>C9+G10</f>
-        <v>36.299999999999997</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
       </c>
       <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f>3212.3*C9</f>
         <v>3212.3</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="1">
+        <f>1*C10</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f>E11+D10</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>7.95</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10" s="1">
         <v>2.83</v>
       </c>
-      <c r="F10" s="1">
+      <c r="H10" s="1">
         <v>8.75</v>
       </c>
-      <c r="G10" s="1">
-        <f>C10</f>
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
+        <f>100.64*C10</f>
         <v>100.64</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="1"/>
     </row>
   </sheetData>
@@ -11526,11 +11576,118 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82230D03-D6E7-494D-8D5E-D2E1D0E431ED}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1">
+        <v>65.5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F923E49D-3BBC-49B4-9B07-9E9EA57DE157}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11554,127 +11711,100 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>13</v>
+        <v>8.75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
-        <v>65.5</v>
+        <v>22000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="1">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="B4" s="6">
+        <v>31.5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.15</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1">
-        <v>8.75</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1">
-        <v>13000</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="6">
-        <f>79300000000</f>
-        <v>79300000000</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="6">
-        <f>210000000000</f>
-        <v>210000000000</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="1">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
+      <c r="G9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060F0E97-B26E-41BD-8C4D-CF7A3B7EAA00}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>